<commit_message>
Changed interval standard 10 days to single days
</commit_message>
<xml_diff>
--- a/sorted_maintenance_tasks.xlsx
+++ b/sorted_maintenance_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramv\Documents\MaintenanceECOFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE978696-6068-4F59-8799-3DE4332B2143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99107DEA-5D7D-4B22-BDBF-42E8FF587514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,30 +78,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -406,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +413,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -435,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -443,311 +429,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
         <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now with total maintenance time per day
</commit_message>
<xml_diff>
--- a/sorted_maintenance_tasks.xlsx
+++ b/sorted_maintenance_tasks.xlsx
@@ -8,31 +8,68 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramv\Documents\MaintenanceECOFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99107DEA-5D7D-4B22-BDBF-42E8FF587514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C613D-09B2-4AA1-BC42-0E94E70B2392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Task Number</t>
   </si>
   <si>
     <t>Interval (Days)</t>
+  </si>
+  <si>
+    <t>0620000-00-01</t>
+  </si>
+  <si>
+    <t>0620000-00-02</t>
+  </si>
+  <si>
+    <t>0620000-00-03</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Menhours</t>
+  </si>
+  <si>
+    <t>0620000-00-04</t>
+  </si>
+  <si>
+    <t>0620000-00-05</t>
+  </si>
+  <si>
+    <t>0620000-00-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,6 +83,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -55,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -78,16 +121,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -392,47 +449,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new tasklist (still a selection)
</commit_message>
<xml_diff>
--- a/sorted_maintenance_tasks.xlsx
+++ b/sorted_maintenance_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramv\Documents\MaintenanceECOFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C613D-09B2-4AA1-BC42-0E94E70B2392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D6D26A-123D-4AC2-A739-A50CD66270B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Task Number</t>
   </si>
@@ -41,28 +41,55 @@
     <t>Interval (Days)</t>
   </si>
   <si>
-    <t>0620000-00-01</t>
-  </si>
-  <si>
-    <t>0620000-00-02</t>
-  </si>
-  <si>
-    <t>0620000-00-03</t>
-  </si>
-  <si>
     <t>Men</t>
   </si>
   <si>
     <t>Menhours</t>
   </si>
   <si>
-    <t>0620000-00-04</t>
-  </si>
-  <si>
-    <t>0620000-00-05</t>
-  </si>
-  <si>
-    <t>0620000-00-06</t>
+    <t>524504-50-01</t>
+  </si>
+  <si>
+    <t>212700-00-01</t>
+  </si>
+  <si>
+    <t>262400-00-02</t>
+  </si>
+  <si>
+    <t>335000-02-04</t>
+  </si>
+  <si>
+    <t>342200-00-01</t>
+  </si>
+  <si>
+    <t>341100-50-01</t>
+  </si>
+  <si>
+    <t>494000-00-01</t>
+  </si>
+  <si>
+    <t>521102-00-09</t>
+  </si>
+  <si>
+    <t>801000-00-02</t>
+  </si>
+  <si>
+    <t>531019-00-05</t>
+  </si>
+  <si>
+    <t>062403-00-01</t>
+  </si>
+  <si>
+    <t>215000-00-09</t>
+  </si>
+  <si>
+    <t>241000-00-02</t>
+  </si>
+  <si>
+    <t>254201-00-01</t>
+  </si>
+  <si>
+    <t>255100-00-01</t>
   </si>
 </sst>
 </file>
@@ -98,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,31 +148,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,18 +475,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -485,12 +495,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>365</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -499,12 +509,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>365</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -513,26 +523,26 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
-        <v>10</v>
+      <c r="B5">
+        <v>365</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
-        <v>20</v>
+      <c r="B6">
+        <v>365</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -541,18 +551,194 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
-        <v>21</v>
+      <c r="B7">
+        <v>365</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>ROUNDDOWN(1000/14,0)</f>
+        <v>71</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f>ROUNDDOWN(1000/13,0)</f>
+        <v>76</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B18" si="0">ROUNDDOWN(1000/13,0)</f>
+        <v>76</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f>ROUNDDOWN(1000/13,0)</f>
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aantal dingen toegevoegd,, als je wilt weten wat, vraag even om te bellen
</commit_message>
<xml_diff>
--- a/sorted_maintenance_tasks.xlsx
+++ b/sorted_maintenance_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramv\Documents\MaintenanceECOFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C876FE-0057-4C21-B121-97C2559263F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79919591-8989-4185-9FAE-47B69AA72B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2489,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A834" workbookViewId="0">
-      <selection activeCell="Q854" sqref="Q854"/>
+    <sheetView tabSelected="1" topLeftCell="A783" workbookViewId="0">
+      <selection activeCell="H821" sqref="H821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2945,7 +2945,7 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3519,7 +3519,7 @@
         <v>165</v>
       </c>
       <c r="B74">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -3995,7 +3995,7 @@
         <v>177</v>
       </c>
       <c r="B108">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -4009,7 +4009,7 @@
         <v>177</v>
       </c>
       <c r="B109">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -4023,7 +4023,7 @@
         <v>178</v>
       </c>
       <c r="B110">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -4079,7 +4079,7 @@
         <v>181</v>
       </c>
       <c r="B114">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -4093,7 +4093,7 @@
         <v>182</v>
       </c>
       <c r="B115">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -4107,7 +4107,7 @@
         <v>183</v>
       </c>
       <c r="B116">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -6053,7 +6053,7 @@
         <v>294</v>
       </c>
       <c r="B255">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -6067,7 +6067,7 @@
         <v>295</v>
       </c>
       <c r="B256">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -6081,7 +6081,7 @@
         <v>296</v>
       </c>
       <c r="B257">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -6095,7 +6095,7 @@
         <v>296</v>
       </c>
       <c r="B258">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -6109,7 +6109,7 @@
         <v>297</v>
       </c>
       <c r="B259">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="C259">
         <v>2</v>
@@ -9749,7 +9749,7 @@
         <v>514</v>
       </c>
       <c r="B519">
-        <v>500</v>
+        <v>444</v>
       </c>
       <c r="C519">
         <v>1</v>
@@ -9763,7 +9763,7 @@
         <v>514</v>
       </c>
       <c r="B520">
-        <v>500</v>
+        <v>444</v>
       </c>
       <c r="C520">
         <v>1</v>
@@ -9777,7 +9777,7 @@
         <v>515</v>
       </c>
       <c r="B521">
-        <v>500</v>
+        <v>444</v>
       </c>
       <c r="C521">
         <v>1</v>
@@ -9791,7 +9791,7 @@
         <v>515</v>
       </c>
       <c r="B522">
-        <v>500</v>
+        <v>444</v>
       </c>
       <c r="C522">
         <v>1</v>
@@ -10085,7 +10085,7 @@
         <v>532</v>
       </c>
       <c r="B543">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="C543">
         <v>1</v>
@@ -10099,7 +10099,7 @@
         <v>532</v>
       </c>
       <c r="B544">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="C544">
         <v>1</v>
@@ -10169,7 +10169,7 @@
         <v>536</v>
       </c>
       <c r="B549">
-        <v>700</v>
+        <v>666</v>
       </c>
       <c r="C549">
         <v>1</v>
@@ -10183,7 +10183,7 @@
         <v>537</v>
       </c>
       <c r="B550">
-        <v>730</v>
+        <v>666</v>
       </c>
       <c r="C550">
         <v>1</v>
@@ -10197,7 +10197,7 @@
         <v>538</v>
       </c>
       <c r="B551">
-        <v>730</v>
+        <v>666</v>
       </c>
       <c r="C551">
         <v>1</v>
@@ -10211,7 +10211,7 @@
         <v>538</v>
       </c>
       <c r="B552">
-        <v>730</v>
+        <v>666</v>
       </c>
       <c r="C552">
         <v>1</v>
@@ -11401,7 +11401,7 @@
         <v>545</v>
       </c>
       <c r="B637">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="C637">
         <v>1</v>
@@ -11415,7 +11415,7 @@
         <v>545</v>
       </c>
       <c r="B638">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="C638">
         <v>1</v>
@@ -13529,7 +13529,7 @@
         <v>670</v>
       </c>
       <c r="B789">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="C789">
         <v>1</v>
@@ -13543,7 +13543,7 @@
         <v>670</v>
       </c>
       <c r="B790">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="C790">
         <v>1</v>
@@ -13767,7 +13767,7 @@
         <v>685</v>
       </c>
       <c r="B806">
-        <v>1500</v>
+        <v>1460</v>
       </c>
       <c r="C806">
         <v>1</v>
@@ -13781,7 +13781,7 @@
         <v>686</v>
       </c>
       <c r="B807">
-        <v>1500</v>
+        <v>1460</v>
       </c>
       <c r="C807">
         <v>1</v>
@@ -13795,7 +13795,7 @@
         <v>687</v>
       </c>
       <c r="B808">
-        <v>1555</v>
+        <v>1460</v>
       </c>
       <c r="C808">
         <v>1</v>
@@ -13823,7 +13823,7 @@
         <v>689</v>
       </c>
       <c r="B810">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C810">
         <v>1</v>
@@ -13837,7 +13837,7 @@
         <v>690</v>
       </c>
       <c r="B811">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C811">
         <v>1</v>
@@ -13851,7 +13851,7 @@
         <v>691</v>
       </c>
       <c r="B812">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C812">
         <v>1</v>
@@ -13865,7 +13865,7 @@
         <v>692</v>
       </c>
       <c r="B813">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C813">
         <v>1</v>
@@ -13879,7 +13879,7 @@
         <v>693</v>
       </c>
       <c r="B814">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C814">
         <v>1</v>
@@ -13893,7 +13893,7 @@
         <v>694</v>
       </c>
       <c r="B815">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C815">
         <v>1</v>
@@ -13907,7 +13907,7 @@
         <v>695</v>
       </c>
       <c r="B816">
-        <v>1825</v>
+        <v>1800</v>
       </c>
       <c r="C816">
         <v>1</v>

</xml_diff>